<commit_message>
Part III finished adjaceny and target tests passed
</commit_message>
<xml_diff>
--- a/Clue_LayoutTestLocationsForPartII.xlsx
+++ b/Clue_LayoutTestLocationsForPartII.xlsx
@@ -534,7 +534,7 @@
   <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA15" sqref="AA15"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1154,7 +1154,7 @@
       <c r="S8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T8" s="6" t="s">
+      <c r="T8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="U8" s="1" t="s">
@@ -1861,7 +1861,7 @@
       <c r="G18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I18" s="1" t="s">

</xml_diff>